<commit_message>
parsing and changes values
</commit_message>
<xml_diff>
--- a/importExample.xlsx
+++ b/importExample.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Arco30\прайсы\Для Загрузки\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OSPanel\domains\xlsBitrixParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B2A9BB1-AC67-4F5B-9EB1-511583ABD331}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{10465894-B61E-49FD-A73A-CD965BC8FBDB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,10 +401,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364E9D03-A225-46D2-A768-F4D41A02A101}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="C315" sqref="C315"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3871,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="C315">
-        <v>38.83</v>
+        <v>38.840000000000003</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -3937,7 +3938,7 @@
         <v>576</v>
       </c>
       <c r="C321">
-        <v>14.03</v>
+        <v>14.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>